<commit_message>
topic 1 last updates
</commit_message>
<xml_diff>
--- a/topic_1_img/topic_1_ex_template.xlsx
+++ b/topic_1_img/topic_1_ex_template.xlsx
@@ -1027,13 +1027,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>142920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>350640</xdr:colOff>
+      <xdr:colOff>350280</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1043,7 +1043,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="142920" y="209520"/>
-          <a:ext cx="9409680" cy="1055520"/>
+          <a:ext cx="9409680" cy="1055160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1176,14 +1176,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>379080</xdr:colOff>
+      <xdr:colOff>378720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1193,7 +1193,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="614160" y="162000"/>
-          <a:ext cx="12560760" cy="798120"/>
+          <a:ext cx="12561840" cy="797760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1313,14 +1313,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>26640</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>26280</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1330,7 +1330,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="614160" y="162000"/>
-          <a:ext cx="17836200" cy="2150640"/>
+          <a:ext cx="17835840" cy="2150280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1554,13 +1554,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>504720</xdr:colOff>
       <xdr:row>168</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1798200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>384840</xdr:colOff>
       <xdr:row>174</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1569,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="504720" y="27866520"/>
-          <a:ext cx="4233600" cy="950400"/>
+          <a:off x="504720" y="29540880"/>
+          <a:ext cx="6012360" cy="1022400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2544,7 +2544,7 @@
       <c r="E30" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="0"/>
+      <c r="H30" s="2"/>
       <c r="J30" s="13" t="s">
         <v>39</v>
       </c>
@@ -2892,7 +2892,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A9:H60"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2904,7 +2904,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="15.23"/>
   </cols>
   <sheetData>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="31" t="s">
         <v>71</v>
       </c>
@@ -3017,11 +3025,16 @@
       <c r="C21" s="38"/>
       <c r="H21" s="35"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="39" t="s">
         <v>85</v>
@@ -3031,14 +3044,14 @@
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="13"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="40" t="s">
         <v>86</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="13"/>
       <c r="C33" s="10" t="s">
         <v>37</v>
@@ -3082,7 +3095,7 @@
       <c r="E33" s="10"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="13"/>
       <c r="C34" s="10" t="s">
         <v>74</v>
@@ -3091,7 +3104,7 @@
       <c r="E34" s="10"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="13"/>
       <c r="C35" s="10" t="s">
         <v>10</v>
@@ -3100,7 +3113,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="13"/>
       <c r="C36" s="10" t="s">
         <v>40</v>
@@ -3109,7 +3122,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="13"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -3128,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="13"/>
       <c r="C39" s="10" t="s">
         <v>45</v>
@@ -3137,7 +3150,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="13"/>
       <c r="C40" s="2" t="s">
         <v>87</v>
@@ -3145,7 +3158,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="13"/>
       <c r="C41" s="10" t="s">
         <v>47</v>
@@ -3154,7 +3167,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="20"/>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="13"/>
       <c r="C42" s="10" t="s">
         <v>49</v>
@@ -3163,7 +3176,7 @@
       <c r="E42" s="10"/>
       <c r="F42" s="20"/>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="13"/>
       <c r="C43" s="10" t="s">
         <v>88</v>
@@ -3172,7 +3185,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="13"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -3191,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="13" t="s">
         <v>55</v>
       </c>
@@ -3203,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="13"/>
       <c r="C47" s="10" t="s">
         <v>73</v>
@@ -3212,7 +3225,7 @@
       <c r="E47" s="10"/>
       <c r="F47" s="20"/>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="13"/>
       <c r="C48" s="10" t="s">
         <v>58</v>
@@ -3221,7 +3234,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13"/>
       <c r="C49" s="10" t="s">
         <v>60</v>
@@ -3230,7 +3243,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="20"/>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13"/>
       <c r="C50" s="10" t="s">
         <v>62</v>
@@ -3239,14 +3252,14 @@
       <c r="E50" s="10"/>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="20"/>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
         <v>5</v>
       </c>
@@ -3258,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13"/>
       <c r="C53" s="10" t="s">
         <v>65</v>
@@ -3267,7 +3280,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="20"/>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13"/>
       <c r="C54" s="10" t="s">
         <v>67</v>
@@ -3276,7 +3289,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="20"/>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13"/>
       <c r="C55" s="2" t="s">
         <v>89</v>
@@ -3285,7 +3298,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="20"/>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -3304,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13"/>
       <c r="C58" s="10" t="s">
         <v>70</v>
@@ -3313,7 +3326,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="20"/>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13"/>
       <c r="C59" s="10" t="s">
         <v>21</v>
@@ -3322,7 +3335,7 @@
       <c r="E59" s="10"/>
       <c r="F59" s="20"/>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="40"/>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -3349,7 +3362,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A7:H39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -3362,7 +3375,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.83"/>
   </cols>
   <sheetData>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="31" t="s">
         <v>71</v>
       </c>
@@ -3370,7 +3389,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="48" t="s">
         <v>91</v>
       </c>
@@ -3378,7 +3397,7 @@
         <v>51692</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="48" t="s">
         <v>92</v>
       </c>
@@ -3386,7 +3405,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="48" t="s">
         <v>93</v>
       </c>
@@ -3394,7 +3413,7 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="48" t="s">
         <v>94</v>
       </c>
@@ -3402,11 +3421,11 @@
         <v>72184</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="48" t="s">
         <v>95</v>
       </c>
@@ -3416,7 +3435,7 @@
       <c r="F13" s="48"/>
       <c r="G13" s="50"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="48" t="s">
         <v>96</v>
       </c>
@@ -3424,7 +3443,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="48" t="s">
         <v>97</v>
       </c>
@@ -3432,7 +3451,7 @@
         <v>16561</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="51" t="s">
         <v>98</v>
       </c>
@@ -3440,11 +3459,14 @@
         <v>72618</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="39" t="s">
         <v>99</v>
@@ -3455,7 +3477,7 @@
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -3463,7 +3485,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="40" t="s">
         <v>32</v>
       </c>
@@ -3475,7 +3497,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="s">
         <v>34</v>
       </c>
@@ -3508,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="13"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -3516,7 +3538,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="13" t="s">
         <v>39</v>
       </c>
@@ -3557,7 +3579,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="46"/>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="13" t="s">
         <v>57</v>
       </c>
@@ -3567,7 +3589,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="13" t="s">
         <v>59</v>
       </c>
@@ -3590,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="13"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -3598,7 +3620,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="13" t="s">
         <v>63</v>
       </c>
@@ -3632,7 +3654,7 @@
       </c>
       <c r="H38" s="56"/>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="40"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -3660,10 +3682,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A16:O183"/>
+  <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D177" activeCellId="0" sqref="D177"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B178" activeCellId="0" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.67578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3676,6 +3698,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="8.94"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="39" t="s">
         <v>102</v>
@@ -3694,7 +3731,7 @@
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -3708,7 +3745,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="40" t="s">
         <v>31</v>
       </c>
@@ -3794,7 +3831,7 @@
         <v>7700</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13"/>
       <c r="C22" s="10" t="s">
         <v>74</v>
@@ -3812,7 +3849,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="20"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13"/>
       <c r="C23" s="10" t="s">
         <v>10</v>
@@ -3832,7 +3869,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13"/>
       <c r="C24" s="10" t="s">
         <v>40</v>
@@ -3850,7 +3887,7 @@
       <c r="L24" s="10"/>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -3891,7 +3928,7 @@
         <v>-1100</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="13"/>
       <c r="C27" s="10" t="s">
         <v>45</v>
@@ -3911,7 +3948,7 @@
       <c r="L27" s="10"/>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="13"/>
       <c r="C28" s="10" t="s">
         <v>47</v>
@@ -3929,7 +3966,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="13"/>
       <c r="C29" s="10" t="s">
         <v>49</v>
@@ -3949,7 +3986,7 @@
         <v>-500</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="13"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -4025,7 +4062,7 @@
       <c r="L33" s="10"/>
       <c r="M33" s="46"/>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="13"/>
       <c r="C34" s="10" t="s">
         <v>73</v>
@@ -4043,7 +4080,7 @@
       <c r="L34" s="10"/>
       <c r="M34" s="20"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="13"/>
       <c r="C35" s="10" t="s">
         <v>58</v>
@@ -4088,7 +4125,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="13"/>
       <c r="C37" s="10" t="s">
         <v>62</v>
@@ -4106,7 +4143,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="20"/>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="13"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -4171,7 +4208,7 @@
         <v>3198.75</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="13"/>
       <c r="C41" s="10" t="s">
         <v>67</v>
@@ -4187,7 +4224,7 @@
       <c r="L41" s="16"/>
       <c r="M41" s="41"/>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="13"/>
       <c r="C42" s="10" t="s">
         <v>68</v>
@@ -4203,7 +4240,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="13"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -4236,7 +4273,7 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="13"/>
       <c r="C45" s="10" t="s">
         <v>70</v>
@@ -4254,7 +4291,7 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="13"/>
       <c r="C46" s="10" t="s">
         <v>21</v>
@@ -4273,7 +4310,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="40"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -4287,12 +4324,13 @@
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
         <v>104</v>
       </c>
@@ -4301,25 +4339,26 @@
       </c>
       <c r="F50" s="57"/>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F51" s="57"/>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F52" s="58"/>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F53" s="58"/>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
         <v>109</v>
       </c>
@@ -4327,7 +4366,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="59" t="s">
         <v>111</v>
       </c>
@@ -4337,7 +4376,7 @@
       <c r="G56" s="59"/>
       <c r="H56" s="59"/>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="59"/>
       <c r="D57" s="59"/>
       <c r="E57" s="59"/>
@@ -4351,7 +4390,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="59"/>
       <c r="D58" s="59"/>
       <c r="E58" s="59"/>
@@ -4359,7 +4398,7 @@
       <c r="G58" s="64"/>
       <c r="H58" s="65"/>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="59"/>
       <c r="D59" s="59"/>
       <c r="E59" s="59"/>
@@ -4367,7 +4406,7 @@
       <c r="G59" s="59"/>
       <c r="H59" s="62"/>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="59" t="s">
         <v>112</v>
       </c>
@@ -4377,7 +4416,7 @@
       <c r="G60" s="59"/>
       <c r="H60" s="62"/>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="59"/>
       <c r="D61" s="59"/>
       <c r="E61" s="59"/>
@@ -4391,7 +4430,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="59"/>
       <c r="D62" s="59"/>
       <c r="E62" s="59"/>
@@ -4399,7 +4438,7 @@
       <c r="G62" s="64"/>
       <c r="H62" s="65"/>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="59"/>
       <c r="D63" s="59"/>
       <c r="E63" s="59"/>
@@ -4407,7 +4446,7 @@
       <c r="G63" s="59"/>
       <c r="H63" s="62"/>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="59" t="s">
         <v>114</v>
       </c>
@@ -4417,7 +4456,7 @@
       <c r="G64" s="59"/>
       <c r="H64" s="62"/>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="59"/>
       <c r="D65" s="59"/>
       <c r="E65" s="59"/>
@@ -4431,7 +4470,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="59"/>
       <c r="D66" s="59"/>
       <c r="E66" s="59"/>
@@ -4439,7 +4478,7 @@
       <c r="G66" s="64"/>
       <c r="H66" s="65"/>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="59"/>
       <c r="D67" s="59"/>
       <c r="E67" s="59"/>
@@ -4447,7 +4486,7 @@
       <c r="G67" s="59"/>
       <c r="H67" s="62"/>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="59"/>
       <c r="D68" s="59"/>
       <c r="E68" s="59"/>
@@ -4455,7 +4494,7 @@
       <c r="G68" s="59"/>
       <c r="H68" s="62"/>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="59" t="s">
         <v>115</v>
       </c>
@@ -4471,7 +4510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
       <c r="E70" s="59"/>
@@ -4479,7 +4518,7 @@
       <c r="G70" s="64"/>
       <c r="H70" s="65"/>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="59"/>
       <c r="D71" s="59"/>
       <c r="E71" s="59"/>
@@ -4513,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
       <c r="E73" s="59"/>
@@ -4521,7 +4560,7 @@
       <c r="G73" s="64"/>
       <c r="H73" s="65"/>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="59"/>
       <c r="D74" s="59"/>
       <c r="E74" s="59"/>
@@ -4545,7 +4584,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="59"/>
       <c r="D76" s="59"/>
       <c r="E76" s="59"/>
@@ -4553,7 +4592,7 @@
       <c r="G76" s="64"/>
       <c r="H76" s="65"/>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="59"/>
       <c r="D77" s="59"/>
       <c r="E77" s="59"/>
@@ -4561,7 +4600,7 @@
       <c r="G77" s="59"/>
       <c r="H77" s="62"/>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="59"/>
       <c r="D78" s="59"/>
       <c r="E78" s="59" t="s">
@@ -4577,7 +4616,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="59"/>
       <c r="D79" s="59"/>
       <c r="E79" s="59"/>
@@ -4585,7 +4624,7 @@
       <c r="G79" s="64"/>
       <c r="H79" s="65"/>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
       <c r="E80" s="59"/>
@@ -4593,11 +4632,12 @@
       <c r="G80" s="59"/>
       <c r="H80" s="59"/>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
         <v>120</v>
       </c>
     </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="39" t="s">
         <v>102</v>
@@ -4616,7 +4656,7 @@
       <c r="L83" s="39"/>
       <c r="M83" s="39"/>
     </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="13"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
@@ -4630,7 +4670,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="14"/>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="40" t="s">
         <v>31</v>
       </c>
@@ -4711,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="13"/>
       <c r="C89" s="10" t="s">
         <v>74</v>
@@ -4727,7 +4767,7 @@
       <c r="L89" s="10"/>
       <c r="M89" s="20"/>
     </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="13"/>
       <c r="C90" s="10" t="s">
         <v>10</v>
@@ -4748,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="13"/>
       <c r="C91" s="10" t="s">
         <v>40</v>
@@ -4766,7 +4806,7 @@
       <c r="L91" s="10"/>
       <c r="M91" s="20"/>
     </row>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="13"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
@@ -4803,7 +4843,7 @@
       <c r="L93" s="10"/>
       <c r="M93" s="20"/>
     </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="13"/>
       <c r="C94" s="10" t="s">
         <v>45</v>
@@ -4821,7 +4861,7 @@
       <c r="L94" s="10"/>
       <c r="M94" s="14"/>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="13"/>
       <c r="C95" s="10" t="s">
         <v>47</v>
@@ -4839,7 +4879,7 @@
       <c r="L95" s="10"/>
       <c r="M95" s="14"/>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="13"/>
       <c r="C96" s="10" t="s">
         <v>49</v>
@@ -4857,7 +4897,7 @@
       <c r="L96" s="10"/>
       <c r="M96" s="20"/>
     </row>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="13"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
@@ -4932,7 +4972,7 @@
       <c r="L100" s="10"/>
       <c r="M100" s="46"/>
     </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="13"/>
       <c r="C101" s="10" t="s">
         <v>73</v>
@@ -4950,7 +4990,7 @@
       <c r="L101" s="10"/>
       <c r="M101" s="20"/>
     </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="13"/>
       <c r="C102" s="10" t="s">
         <v>58</v>
@@ -4989,7 +5029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="13"/>
       <c r="C104" s="10" t="s">
         <v>62</v>
@@ -5005,7 +5045,7 @@
       <c r="L104" s="10"/>
       <c r="M104" s="20"/>
     </row>
-    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="13"/>
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
@@ -5069,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="13"/>
       <c r="C108" s="10" t="s">
         <v>67</v>
@@ -5085,7 +5125,7 @@
       <c r="L108" s="16"/>
       <c r="M108" s="41"/>
     </row>
-    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="13"/>
       <c r="C109" s="10" t="s">
         <v>68</v>
@@ -5101,7 +5141,7 @@
       <c r="L109" s="10"/>
       <c r="M109" s="10"/>
     </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="13"/>
       <c r="C110" s="10"/>
       <c r="D110" s="10"/>
@@ -5134,7 +5174,7 @@
       <c r="L111" s="10"/>
       <c r="M111" s="10"/>
     </row>
-    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="13"/>
       <c r="C112" s="10" t="s">
         <v>70</v>
@@ -5150,7 +5190,7 @@
       <c r="L112" s="10"/>
       <c r="M112" s="10"/>
     </row>
-    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="13"/>
       <c r="C113" s="10" t="s">
         <v>21</v>
@@ -5166,7 +5206,7 @@
       <c r="L113" s="10"/>
       <c r="M113" s="10"/>
     </row>
-    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="40"/>
       <c r="C114" s="16"/>
       <c r="D114" s="16"/>
@@ -5180,7 +5220,9 @@
       <c r="L114" s="10"/>
       <c r="M114" s="10"/>
     </row>
-    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="2" t="s">
         <v>105</v>
       </c>
@@ -5189,7 +5231,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="2" t="s">
         <v>106</v>
       </c>
@@ -5198,7 +5240,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="2" t="s">
         <v>107</v>
       </c>
@@ -5207,7 +5249,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="2" t="s">
         <v>108</v>
       </c>
@@ -5216,11 +5258,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
         <v>121</v>
       </c>
     </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
         <v>102</v>
@@ -5239,7 +5282,7 @@
       <c r="L123" s="39"/>
       <c r="M123" s="39"/>
     </row>
-    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="13"/>
       <c r="C124" s="10"/>
       <c r="D124" s="10"/>
@@ -5253,7 +5296,7 @@
       <c r="L124" s="10"/>
       <c r="M124" s="14"/>
     </row>
-    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="40" t="s">
         <v>31</v>
       </c>
@@ -5334,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="13"/>
       <c r="C129" s="10" t="s">
         <v>74</v>
@@ -5350,7 +5393,7 @@
       <c r="L129" s="10"/>
       <c r="M129" s="20"/>
     </row>
-    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="13"/>
       <c r="C130" s="10" t="s">
         <v>10</v>
@@ -5371,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="13"/>
       <c r="C131" s="10" t="s">
         <v>40</v>
@@ -5389,7 +5432,7 @@
       <c r="L131" s="10"/>
       <c r="M131" s="20"/>
     </row>
-    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="13"/>
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
@@ -5426,7 +5469,7 @@
       <c r="L133" s="10"/>
       <c r="M133" s="20"/>
     </row>
-    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="13"/>
       <c r="C134" s="10" t="s">
         <v>45</v>
@@ -5444,7 +5487,7 @@
       <c r="L134" s="10"/>
       <c r="M134" s="14"/>
     </row>
-    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="13"/>
       <c r="C135" s="10" t="s">
         <v>47</v>
@@ -5462,7 +5505,7 @@
       <c r="L135" s="10"/>
       <c r="M135" s="14"/>
     </row>
-    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="13"/>
       <c r="C136" s="10" t="s">
         <v>49</v>
@@ -5480,7 +5523,7 @@
       <c r="L136" s="10"/>
       <c r="M136" s="20"/>
     </row>
-    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="13"/>
       <c r="C137" s="10"/>
       <c r="D137" s="10"/>
@@ -5555,7 +5598,7 @@
       <c r="L140" s="10"/>
       <c r="M140" s="46"/>
     </row>
-    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="13"/>
       <c r="C141" s="10" t="s">
         <v>73</v>
@@ -5573,7 +5616,7 @@
       <c r="L141" s="10"/>
       <c r="M141" s="20"/>
     </row>
-    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="13"/>
       <c r="C142" s="10" t="s">
         <v>58</v>
@@ -5612,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="13"/>
       <c r="C144" s="10" t="s">
         <v>62</v>
@@ -5628,7 +5671,7 @@
       <c r="L144" s="10"/>
       <c r="M144" s="20"/>
     </row>
-    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="13"/>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
@@ -5692,7 +5735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="13"/>
       <c r="C148" s="10" t="s">
         <v>67</v>
@@ -5708,7 +5751,7 @@
       <c r="L148" s="16"/>
       <c r="M148" s="41"/>
     </row>
-    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="13"/>
       <c r="C149" s="10" t="s">
         <v>68</v>
@@ -5724,7 +5767,7 @@
       <c r="L149" s="10"/>
       <c r="M149" s="10"/>
     </row>
-    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="13"/>
       <c r="C150" s="10"/>
       <c r="D150" s="10"/>
@@ -5757,7 +5800,7 @@
       <c r="L151" s="10"/>
       <c r="M151" s="10"/>
     </row>
-    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="13"/>
       <c r="C152" s="10" t="s">
         <v>70</v>
@@ -5773,7 +5816,7 @@
       <c r="L152" s="10"/>
       <c r="M152" s="10"/>
     </row>
-    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="13"/>
       <c r="C153" s="10" t="s">
         <v>21</v>
@@ -5789,7 +5832,7 @@
       <c r="L153" s="10"/>
       <c r="M153" s="10"/>
     </row>
-    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="40"/>
       <c r="C154" s="16"/>
       <c r="D154" s="16"/>
@@ -5803,7 +5846,9 @@
       <c r="L154" s="10"/>
       <c r="M154" s="10"/>
     </row>
-    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="2" t="s">
         <v>105</v>
       </c>
@@ -5812,7 +5857,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="2" t="s">
         <v>106</v>
       </c>
@@ -5821,7 +5866,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="2" t="s">
         <v>107</v>
       </c>
@@ -5830,7 +5875,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="2" t="s">
         <v>108</v>
       </c>
@@ -5839,13 +5884,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="31"/>
       <c r="C162" s="31"/>
       <c r="D162" s="31"/>
       <c r="E162" s="31"/>
     </row>
-    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="31" t="s">
         <v>122</v>
       </c>
@@ -5859,7 +5905,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="2" t="s">
         <v>105</v>
       </c>
@@ -5876,7 +5922,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="2" t="s">
         <v>125</v>
       </c>
@@ -5893,7 +5939,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="2" t="s">
         <v>107</v>
       </c>
@@ -5910,7 +5956,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="31" t="s">
         <v>108</v>
       </c>
@@ -5927,7 +5973,22 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="2" t="s">
         <v>126</v>
       </c>

</xml_diff>